<commit_message>
tests : concentrations : xlsx
</commit_message>
<xml_diff>
--- a/tests/data.gui/test/concentrations/ds.1p/kev.concentrations.data.xlsx
+++ b/tests/data.gui/test/concentrations/ds.1p/kev.concentrations.data.xlsx
@@ -9,10 +9,11 @@
     <sheet name="input_stoich_coefficients" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="input_k_constants_log10" sheetId="2" state="visible" r:id="rId2"/>
     <sheet name="input_concentrations" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="equilibrium_concentrations" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet name="Cu_fractions" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet name="percent_error" sheetId="6" state="visible" r:id="rId6"/>
-    <sheet name="component_names" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet name="total_concentrations" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="equilibrium_concentrations" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="Cu_fractions" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="percent_error" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet name="component_names" sheetId="8" state="visible" r:id="rId8"/>
   </sheets>
 </workbook>
 </file>
@@ -504,6 +505,36 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="B2" t="n">
+        <v>0.02</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
         <v>6</v>
       </c>
       <c r="B1" t="s">
@@ -536,7 +567,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
@@ -578,7 +609,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
@@ -608,7 +639,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>

</xml_diff>